<commit_message>
add AudioUrls for Record
</commit_message>
<xml_diff>
--- a/src/test/resources/topics/Классификатор методики МИЦИАР.xlsx
+++ b/src/test/resources/topics/Классификатор методики МИЦИАР.xlsx
@@ -18,6 +18,12 @@
     <author/>
   </authors>
   <commentList>
+    <comment authorId="0" ref="B220">
+      <text>
+        <t xml:space="preserve">сократить
+	-Сллóуйссгóрт Смаай-Гррийсс</t>
+      </text>
+    </comment>
     <comment authorId="0" ref="C453">
       <text>
         <t xml:space="preserve">что значит понятие? :)
@@ -254,7 +260,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1301" uniqueCount="1279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1304" uniqueCount="1281">
   <si>
     <t>СТРУКТУРА МЕТОДИКИ МИЦИАР</t>
   </si>
@@ -660,7 +666,7 @@
       <rPr>
         <color rgb="FFFF00FF"/>
       </rPr>
-      <t>140-1</t>
+      <t>140-1, 152-3,</t>
     </r>
   </si>
   <si>
@@ -709,7 +715,10 @@
       <rPr>
         <color rgb="FF0000FF"/>
       </rPr>
-      <t>82-2,96-2, 123-2</t>
+      <t xml:space="preserve">82-2,96-2, 123-2, </t>
+    </r>
+    <r>
+      <t xml:space="preserve">152 1, </t>
     </r>
   </si>
   <si>
@@ -1280,7 +1289,7 @@
     <t>WE</t>
   </si>
   <si>
-    <t>ИИССИИДИ-Центры и комплиментарной системе (общая инфо, что это такое)</t>
+    <t>ИИССИИДИ-Центры и комплиментарная система (общая информация)</t>
   </si>
   <si>
     <t>UZ</t>
@@ -2126,7 +2135,7 @@
       <rPr>
         <color rgb="FFFF00FF"/>
       </rPr>
-      <t>12-1, 153-1,</t>
+      <t>12-1, 153-1, 154-2,</t>
     </r>
   </si>
   <si>
@@ -2160,7 +2169,7 @@
       <rPr>
         <color rgb="FFFF00FF"/>
       </rPr>
-      <t xml:space="preserve"> 140-3, 12-1,</t>
+      <t xml:space="preserve"> 140-3, 12-1, 154-2,</t>
     </r>
   </si>
   <si>
@@ -2312,7 +2321,7 @@
     <t>Эмоциональный интеллект</t>
   </si>
   <si>
-    <t>НУУЛЛ-ВВУ, как Образ человека, лишённого активности первых 4-ёх Уровней первых двух ИИ-Центров</t>
+    <t>НУУЛЛ-ВВУ, как Образ человека, лишённого активности первых 4-ёх Уровней первых двух ИИ-Центров.НУУЛЛ-ВВУ как Эталон для ориентации направлений перефокусировок и Образ для работы с методиками</t>
   </si>
   <si>
     <t>PV</t>
@@ -2465,7 +2474,7 @@
     <t>OB</t>
   </si>
   <si>
-    <t>15-2, 140-3,</t>
+    <t>15-2, 140-3, 152-2,</t>
   </si>
   <si>
     <t>Возможно дублирование данного пункта в "практиках и методиках"</t>
@@ -2535,7 +2544,7 @@
       <t xml:space="preserve"> 148-1, </t>
     </r>
     <r>
-      <t>153-3,</t>
+      <t xml:space="preserve">153-3, 152-1, </t>
     </r>
   </si>
   <si>
@@ -4411,6 +4420,9 @@
     <t>CX</t>
   </si>
   <si>
+    <t xml:space="preserve">156-3, </t>
+  </si>
+  <si>
     <t>Роль вирусов в процессе перефокусировок</t>
   </si>
   <si>
@@ -4708,6 +4720,9 @@
   </si>
   <si>
     <t>319-1, 320-3</t>
+  </si>
+  <si>
+    <t>О пище будущего</t>
   </si>
 </sst>
 </file>
@@ -5197,7 +5212,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="175">
+  <cellXfs count="176">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -5628,6 +5643,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="69" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="48" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="48" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -13348,7 +13366,9 @@
       <c r="H498" s="108" t="s">
         <v>1189</v>
       </c>
-      <c r="I498" s="135"/>
+      <c r="I498" s="147" t="s">
+        <v>1190</v>
+      </c>
       <c r="J498" s="110"/>
       <c r="K498" s="111"/>
       <c r="L498" s="104"/>
@@ -13357,10 +13377,10 @@
       <c r="A499" s="112"/>
       <c r="B499" s="28"/>
       <c r="C499" s="29" t="s">
-        <v>1190</v>
+        <v>1191</v>
       </c>
       <c r="H499" s="108" t="s">
-        <v>1191</v>
+        <v>1192</v>
       </c>
       <c r="I499" s="135"/>
       <c r="J499" s="110"/>
@@ -13371,10 +13391,10 @@
       <c r="A500" s="112"/>
       <c r="B500" s="28"/>
       <c r="C500" s="29" t="s">
-        <v>1192</v>
+        <v>1193</v>
       </c>
       <c r="H500" s="108" t="s">
-        <v>1193</v>
+        <v>1194</v>
       </c>
       <c r="I500" s="135"/>
       <c r="J500" s="110"/>
@@ -13385,10 +13405,10 @@
       <c r="A501" s="112"/>
       <c r="B501" s="28"/>
       <c r="C501" s="49" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="H501" s="108" t="s">
-        <v>1195</v>
+        <v>1196</v>
       </c>
       <c r="I501" s="135"/>
       <c r="J501" s="110"/>
@@ -13398,13 +13418,13 @@
     <row r="502" ht="15.75" customHeight="1">
       <c r="A502" s="112"/>
       <c r="B502" s="32" t="s">
-        <v>1196</v>
+        <v>1197</v>
       </c>
       <c r="H502" s="108" t="s">
-        <v>1197</v>
-      </c>
-      <c r="I502" s="147" t="s">
         <v>1198</v>
+      </c>
+      <c r="I502" s="148" t="s">
+        <v>1199</v>
       </c>
       <c r="J502" s="110"/>
       <c r="K502" s="111"/>
@@ -13414,12 +13434,12 @@
       <c r="A503" s="112"/>
       <c r="B503" s="28"/>
       <c r="C503" s="29" t="s">
-        <v>1199</v>
+        <v>1200</v>
       </c>
       <c r="H503" s="108" t="s">
-        <v>1200</v>
-      </c>
-      <c r="I503" s="148"/>
+        <v>1201</v>
+      </c>
+      <c r="I503" s="149"/>
       <c r="J503" s="110"/>
       <c r="K503" s="111"/>
       <c r="L503" s="104"/>
@@ -13428,10 +13448,10 @@
       <c r="A504" s="112"/>
       <c r="B504" s="28"/>
       <c r="C504" s="29" t="s">
-        <v>1201</v>
+        <v>1202</v>
       </c>
       <c r="H504" s="108" t="s">
-        <v>1202</v>
+        <v>1203</v>
       </c>
       <c r="I504" s="135"/>
       <c r="J504" s="110"/>
@@ -13442,10 +13462,10 @@
       <c r="A505" s="112"/>
       <c r="B505" s="28"/>
       <c r="C505" s="29" t="s">
-        <v>1203</v>
+        <v>1204</v>
       </c>
       <c r="H505" s="108" t="s">
-        <v>1204</v>
+        <v>1205</v>
       </c>
       <c r="I505" s="135"/>
       <c r="J505" s="110"/>
@@ -13456,13 +13476,13 @@
       <c r="A506" s="112"/>
       <c r="B506" s="28"/>
       <c r="C506" s="29" t="s">
-        <v>1205</v>
+        <v>1206</v>
       </c>
       <c r="H506" s="108" t="s">
-        <v>1206</v>
+        <v>1207</v>
       </c>
       <c r="I506" s="141" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="J506" s="110"/>
       <c r="K506" s="111"/>
@@ -13472,28 +13492,28 @@
       <c r="A507" s="112"/>
       <c r="B507" s="28"/>
       <c r="C507" s="29" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="H507" s="108" t="s">
-        <v>1209</v>
+        <v>1210</v>
       </c>
       <c r="I507" s="135"/>
       <c r="J507" s="110"/>
       <c r="K507" s="111" t="s">
-        <v>1210</v>
+        <v>1211</v>
       </c>
       <c r="L507" s="104"/>
     </row>
     <row r="508" ht="15.75" customHeight="1">
       <c r="A508" s="112"/>
       <c r="B508" s="32" t="s">
-        <v>1211</v>
+        <v>1212</v>
       </c>
       <c r="H508" s="108" t="s">
-        <v>1212</v>
+        <v>1213</v>
       </c>
       <c r="I508" s="116" t="s">
-        <v>1213</v>
+        <v>1214</v>
       </c>
       <c r="J508" s="110"/>
       <c r="K508" s="111"/>
@@ -13502,10 +13522,10 @@
     <row r="509" ht="15.75" customHeight="1">
       <c r="A509" s="112"/>
       <c r="B509" s="32" t="s">
-        <v>1214</v>
+        <v>1215</v>
       </c>
       <c r="H509" s="108" t="s">
-        <v>1215</v>
+        <v>1216</v>
       </c>
       <c r="I509" s="135"/>
       <c r="J509" s="110"/>
@@ -13515,10 +13535,10 @@
     <row r="510" ht="15.75" customHeight="1">
       <c r="A510" s="119"/>
       <c r="B510" s="32" t="s">
-        <v>1216</v>
+        <v>1217</v>
       </c>
       <c r="H510" s="108" t="s">
-        <v>1217</v>
+        <v>1218</v>
       </c>
       <c r="I510" s="135"/>
       <c r="J510" s="110"/>
@@ -13528,13 +13548,13 @@
     <row r="511" ht="15.75" customHeight="1">
       <c r="A511" s="112"/>
       <c r="B511" s="32" t="s">
-        <v>1218</v>
+        <v>1219</v>
       </c>
       <c r="H511" s="108" t="s">
-        <v>1219</v>
+        <v>1220</v>
       </c>
       <c r="I511" s="137" t="s">
-        <v>1220</v>
+        <v>1221</v>
       </c>
       <c r="J511" s="110"/>
       <c r="K511" s="111"/>
@@ -13543,10 +13563,10 @@
     <row r="512" ht="15.75" customHeight="1">
       <c r="A512" s="112"/>
       <c r="B512" s="32" t="s">
-        <v>1221</v>
+        <v>1222</v>
       </c>
       <c r="H512" s="108" t="s">
-        <v>1222</v>
+        <v>1223</v>
       </c>
       <c r="I512" s="135"/>
       <c r="J512" s="110"/>
@@ -13556,10 +13576,10 @@
     <row r="513" ht="15.75" customHeight="1">
       <c r="A513" s="112"/>
       <c r="B513" s="32" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="H513" s="108" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="I513" s="133"/>
       <c r="J513" s="134"/>
@@ -13569,10 +13589,10 @@
     <row r="514" ht="15.75" customHeight="1">
       <c r="A514" s="112"/>
       <c r="B514" s="32" t="s">
-        <v>1225</v>
+        <v>1226</v>
       </c>
       <c r="H514" s="108" t="s">
-        <v>1226</v>
+        <v>1227</v>
       </c>
       <c r="I514" s="133"/>
       <c r="J514" s="134"/>
@@ -13582,13 +13602,13 @@
     <row r="515" ht="15.75" customHeight="1">
       <c r="A515" s="112"/>
       <c r="B515" s="32" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
       <c r="H515" s="108" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
       <c r="I515" s="145" t="s">
-        <v>1229</v>
+        <v>1230</v>
       </c>
       <c r="J515" s="134"/>
       <c r="K515" s="111"/>
@@ -13597,10 +13617,10 @@
     <row r="516" ht="15.75" customHeight="1">
       <c r="A516" s="112"/>
       <c r="B516" s="32" t="s">
-        <v>1230</v>
+        <v>1231</v>
       </c>
       <c r="H516" s="108" t="s">
-        <v>1231</v>
+        <v>1232</v>
       </c>
       <c r="I516" s="134"/>
       <c r="J516" s="134"/>
@@ -13610,7 +13630,7 @@
     <row r="517" ht="15.75" customHeight="1">
       <c r="A517" s="112"/>
       <c r="B517" s="32" t="s">
-        <v>1232</v>
+        <v>1233</v>
       </c>
       <c r="H517" s="117"/>
       <c r="I517" s="134"/>
@@ -13628,321 +13648,321 @@
       <c r="L518" s="104"/>
     </row>
     <row r="519" ht="15.75" customHeight="1">
-      <c r="A519" s="149" t="s">
-        <v>1233</v>
-      </c>
-      <c r="B519" s="150"/>
-      <c r="C519" s="150"/>
-      <c r="D519" s="150"/>
-      <c r="E519" s="150"/>
-      <c r="F519" s="150"/>
-      <c r="G519" s="150"/>
-      <c r="H519" s="151"/>
+      <c r="A519" s="150" t="s">
+        <v>1234</v>
+      </c>
+      <c r="B519" s="151"/>
+      <c r="C519" s="151"/>
+      <c r="D519" s="151"/>
+      <c r="E519" s="151"/>
+      <c r="F519" s="151"/>
+      <c r="G519" s="151"/>
+      <c r="H519" s="152"/>
       <c r="I519" s="134"/>
       <c r="J519" s="134"/>
       <c r="K519" s="111"/>
       <c r="L519" s="104"/>
     </row>
     <row r="520" ht="15.75" customHeight="1">
-      <c r="A520" s="152" t="s">
-        <v>1234</v>
-      </c>
-      <c r="B520" s="153"/>
-      <c r="C520" s="154"/>
-      <c r="D520" s="154"/>
-      <c r="E520" s="154"/>
-      <c r="F520" s="154"/>
-      <c r="G520" s="154"/>
-      <c r="I520" s="155" t="s">
+      <c r="A520" s="153" t="s">
         <v>1235</v>
       </c>
-      <c r="J520" s="156"/>
-      <c r="K520" s="156"/>
+      <c r="B520" s="154"/>
+      <c r="C520" s="155"/>
+      <c r="D520" s="155"/>
+      <c r="E520" s="155"/>
+      <c r="F520" s="155"/>
+      <c r="G520" s="155"/>
+      <c r="I520" s="156" t="s">
+        <v>1236</v>
+      </c>
+      <c r="J520" s="157"/>
+      <c r="K520" s="157"/>
     </row>
     <row r="521" ht="15.75" customHeight="1">
-      <c r="A521" s="157" t="s">
-        <v>1236</v>
-      </c>
-      <c r="B521" s="153"/>
-      <c r="C521" s="154"/>
-      <c r="D521" s="154"/>
-      <c r="E521" s="154"/>
-      <c r="F521" s="154"/>
-      <c r="G521" s="154"/>
-      <c r="I521" s="158" t="s">
+      <c r="A521" s="158" t="s">
         <v>1237</v>
       </c>
-      <c r="J521" s="156"/>
-      <c r="K521" s="156"/>
+      <c r="B521" s="154"/>
+      <c r="C521" s="155"/>
+      <c r="D521" s="155"/>
+      <c r="E521" s="155"/>
+      <c r="F521" s="155"/>
+      <c r="G521" s="155"/>
+      <c r="I521" s="159" t="s">
+        <v>1238</v>
+      </c>
+      <c r="J521" s="157"/>
+      <c r="K521" s="157"/>
     </row>
     <row r="522" ht="15.75" customHeight="1">
-      <c r="A522" s="157" t="s">
-        <v>1238</v>
-      </c>
-      <c r="B522" s="153"/>
-      <c r="C522" s="154"/>
-      <c r="D522" s="154"/>
-      <c r="E522" s="154"/>
-      <c r="F522" s="154"/>
-      <c r="G522" s="154"/>
-      <c r="I522" s="159" t="s">
+      <c r="A522" s="158" t="s">
         <v>1239</v>
       </c>
-      <c r="J522" s="156"/>
-      <c r="K522" s="156"/>
+      <c r="B522" s="154"/>
+      <c r="C522" s="155"/>
+      <c r="D522" s="155"/>
+      <c r="E522" s="155"/>
+      <c r="F522" s="155"/>
+      <c r="G522" s="155"/>
+      <c r="I522" s="160" t="s">
+        <v>1240</v>
+      </c>
+      <c r="J522" s="157"/>
+      <c r="K522" s="157"/>
     </row>
     <row r="523" ht="15.75" customHeight="1">
-      <c r="A523" s="157" t="s">
-        <v>1240</v>
-      </c>
-      <c r="B523" s="153"/>
-      <c r="C523" s="154"/>
-      <c r="D523" s="154"/>
-      <c r="E523" s="154"/>
-      <c r="F523" s="154"/>
-      <c r="G523" s="154"/>
-      <c r="I523" s="160" t="s">
+      <c r="A523" s="158" t="s">
         <v>1241</v>
       </c>
-      <c r="J523" s="156"/>
-      <c r="K523" s="156"/>
+      <c r="B523" s="154"/>
+      <c r="C523" s="155"/>
+      <c r="D523" s="155"/>
+      <c r="E523" s="155"/>
+      <c r="F523" s="155"/>
+      <c r="G523" s="155"/>
+      <c r="I523" s="161" t="s">
+        <v>1242</v>
+      </c>
+      <c r="J523" s="157"/>
+      <c r="K523" s="157"/>
     </row>
     <row r="524" ht="15.75" customHeight="1">
-      <c r="A524" s="157" t="s">
-        <v>1242</v>
-      </c>
-      <c r="B524" s="153"/>
-      <c r="C524" s="154"/>
-      <c r="D524" s="154"/>
-      <c r="E524" s="154"/>
-      <c r="F524" s="154"/>
-      <c r="G524" s="154"/>
-      <c r="I524" s="161" t="s">
+      <c r="A524" s="158" t="s">
         <v>1243</v>
       </c>
-      <c r="J524" s="156"/>
-      <c r="K524" s="156"/>
+      <c r="B524" s="154"/>
+      <c r="C524" s="155"/>
+      <c r="D524" s="155"/>
+      <c r="E524" s="155"/>
+      <c r="F524" s="155"/>
+      <c r="G524" s="155"/>
+      <c r="I524" s="162" t="s">
+        <v>1244</v>
+      </c>
+      <c r="J524" s="157"/>
+      <c r="K524" s="157"/>
     </row>
     <row r="525" ht="15.75" customHeight="1">
-      <c r="A525" s="157" t="s">
-        <v>1244</v>
-      </c>
-      <c r="B525" s="153"/>
-      <c r="C525" s="154"/>
-      <c r="D525" s="154"/>
-      <c r="E525" s="154"/>
-      <c r="F525" s="154"/>
-      <c r="G525" s="154"/>
-      <c r="I525" s="162" t="s">
+      <c r="A525" s="158" t="s">
         <v>1245</v>
       </c>
-      <c r="J525" s="156"/>
-      <c r="K525" s="156"/>
+      <c r="B525" s="154"/>
+      <c r="C525" s="155"/>
+      <c r="D525" s="155"/>
+      <c r="E525" s="155"/>
+      <c r="F525" s="155"/>
+      <c r="G525" s="155"/>
+      <c r="I525" s="163" t="s">
+        <v>1246</v>
+      </c>
+      <c r="J525" s="157"/>
+      <c r="K525" s="157"/>
     </row>
     <row r="526" ht="15.75" customHeight="1">
-      <c r="A526" s="163" t="s">
-        <v>1246</v>
-      </c>
-      <c r="B526" s="153"/>
-      <c r="C526" s="154"/>
-      <c r="D526" s="154"/>
-      <c r="E526" s="154"/>
-      <c r="F526" s="154"/>
-      <c r="G526" s="154"/>
-      <c r="I526" s="164" t="s">
+      <c r="A526" s="164" t="s">
         <v>1247</v>
       </c>
-      <c r="J526" s="156"/>
-      <c r="K526" s="156"/>
+      <c r="B526" s="154"/>
+      <c r="C526" s="155"/>
+      <c r="D526" s="155"/>
+      <c r="E526" s="155"/>
+      <c r="F526" s="155"/>
+      <c r="G526" s="155"/>
+      <c r="I526" s="165" t="s">
+        <v>1248</v>
+      </c>
+      <c r="J526" s="157"/>
+      <c r="K526" s="157"/>
     </row>
     <row r="527" ht="15.75" customHeight="1">
-      <c r="A527" s="157" t="s">
-        <v>1248</v>
-      </c>
-      <c r="B527" s="153"/>
-      <c r="C527" s="154"/>
-      <c r="D527" s="154"/>
-      <c r="E527" s="154"/>
-      <c r="F527" s="154"/>
-      <c r="G527" s="154"/>
-      <c r="I527" s="165" t="s">
+      <c r="A527" s="158" t="s">
         <v>1249</v>
       </c>
-      <c r="J527" s="156"/>
-      <c r="K527" s="156"/>
+      <c r="B527" s="154"/>
+      <c r="C527" s="155"/>
+      <c r="D527" s="155"/>
+      <c r="E527" s="155"/>
+      <c r="F527" s="155"/>
+      <c r="G527" s="155"/>
+      <c r="I527" s="166" t="s">
+        <v>1250</v>
+      </c>
+      <c r="J527" s="157"/>
+      <c r="K527" s="157"/>
     </row>
     <row r="528" ht="15.75" customHeight="1">
-      <c r="A528" s="166" t="s">
-        <v>1250</v>
-      </c>
-      <c r="B528" s="166"/>
-      <c r="C528" s="156"/>
-      <c r="D528" s="156"/>
-      <c r="E528" s="156"/>
-      <c r="F528" s="156"/>
-      <c r="G528" s="166"/>
-      <c r="H528" s="156"/>
-      <c r="I528" s="167" t="s">
+      <c r="A528" s="167" t="s">
         <v>1251</v>
       </c>
-      <c r="J528" s="156"/>
-      <c r="K528" s="156"/>
+      <c r="B528" s="167"/>
+      <c r="C528" s="157"/>
+      <c r="D528" s="157"/>
+      <c r="E528" s="157"/>
+      <c r="F528" s="157"/>
+      <c r="G528" s="167"/>
+      <c r="H528" s="157"/>
+      <c r="I528" s="168" t="s">
+        <v>1252</v>
+      </c>
+      <c r="J528" s="157"/>
+      <c r="K528" s="157"/>
     </row>
     <row r="529" ht="15.75" customHeight="1">
-      <c r="A529" s="166" t="s">
-        <v>1252</v>
-      </c>
-      <c r="H529" s="156"/>
-      <c r="I529" s="167" t="s">
+      <c r="A529" s="167" t="s">
         <v>1253</v>
       </c>
-      <c r="J529" s="156"/>
-      <c r="K529" s="156"/>
+      <c r="H529" s="157"/>
+      <c r="I529" s="168" t="s">
+        <v>1254</v>
+      </c>
+      <c r="J529" s="157"/>
+      <c r="K529" s="157"/>
     </row>
     <row r="530" ht="15.75" customHeight="1">
-      <c r="A530" s="166" t="s">
-        <v>1254</v>
-      </c>
-      <c r="H530" s="156"/>
-      <c r="I530" s="168" t="s">
+      <c r="A530" s="167" t="s">
         <v>1255</v>
       </c>
-      <c r="J530" s="156"/>
-      <c r="K530" s="156"/>
+      <c r="H530" s="157"/>
+      <c r="I530" s="169" t="s">
+        <v>1256</v>
+      </c>
+      <c r="J530" s="157"/>
+      <c r="K530" s="157"/>
     </row>
     <row r="531" ht="15.75" customHeight="1">
-      <c r="A531" s="169" t="s">
-        <v>1256</v>
-      </c>
-      <c r="B531" s="170"/>
-      <c r="C531" s="171"/>
-      <c r="D531" s="171"/>
-      <c r="E531" s="171"/>
-      <c r="F531" s="171"/>
-      <c r="G531" s="172"/>
-      <c r="H531" s="156"/>
-      <c r="I531" s="168" t="s">
+      <c r="A531" s="170" t="s">
         <v>1257</v>
       </c>
-      <c r="J531" s="156"/>
-      <c r="K531" s="156"/>
+      <c r="B531" s="171"/>
+      <c r="C531" s="172"/>
+      <c r="D531" s="172"/>
+      <c r="E531" s="172"/>
+      <c r="F531" s="172"/>
+      <c r="G531" s="173"/>
+      <c r="H531" s="157"/>
+      <c r="I531" s="169" t="s">
+        <v>1258</v>
+      </c>
+      <c r="J531" s="157"/>
+      <c r="K531" s="157"/>
     </row>
     <row r="532" ht="15.75" customHeight="1">
-      <c r="A532" s="166" t="s">
-        <v>1258</v>
-      </c>
-      <c r="B532" s="166"/>
-      <c r="C532" s="156"/>
-      <c r="D532" s="156"/>
-      <c r="E532" s="156"/>
-      <c r="F532" s="156"/>
-      <c r="G532" s="156"/>
-      <c r="H532" s="156"/>
-      <c r="I532" s="168" t="s">
+      <c r="A532" s="167" t="s">
         <v>1259</v>
       </c>
-      <c r="J532" s="156"/>
-      <c r="K532" s="156"/>
+      <c r="B532" s="167"/>
+      <c r="C532" s="157"/>
+      <c r="D532" s="157"/>
+      <c r="E532" s="157"/>
+      <c r="F532" s="157"/>
+      <c r="G532" s="157"/>
+      <c r="H532" s="157"/>
+      <c r="I532" s="169" t="s">
+        <v>1260</v>
+      </c>
+      <c r="J532" s="157"/>
+      <c r="K532" s="157"/>
     </row>
     <row r="533" ht="15.75" customHeight="1">
-      <c r="A533" s="166" t="s">
-        <v>1260</v>
-      </c>
-      <c r="B533" s="166"/>
-      <c r="C533" s="156"/>
-      <c r="D533" s="156"/>
-      <c r="E533" s="156"/>
-      <c r="F533" s="156"/>
-      <c r="G533" s="156"/>
-      <c r="H533" s="156"/>
-      <c r="I533" s="168" t="s">
+      <c r="A533" s="167" t="s">
         <v>1261</v>
       </c>
-      <c r="J533" s="156"/>
-      <c r="K533" s="156"/>
+      <c r="B533" s="167"/>
+      <c r="C533" s="157"/>
+      <c r="D533" s="157"/>
+      <c r="E533" s="157"/>
+      <c r="F533" s="157"/>
+      <c r="G533" s="157"/>
+      <c r="H533" s="157"/>
+      <c r="I533" s="169" t="s">
+        <v>1262</v>
+      </c>
+      <c r="J533" s="157"/>
+      <c r="K533" s="157"/>
     </row>
     <row r="534" ht="15.75" customHeight="1">
-      <c r="A534" s="166" t="s">
-        <v>1262</v>
-      </c>
-      <c r="B534" s="166"/>
-      <c r="C534" s="156"/>
-      <c r="D534" s="156"/>
-      <c r="E534" s="156"/>
-      <c r="F534" s="156"/>
-      <c r="G534" s="156"/>
-      <c r="H534" s="156"/>
-      <c r="I534" s="173" t="s">
+      <c r="A534" s="167" t="s">
         <v>1263</v>
       </c>
-      <c r="J534" s="156"/>
-      <c r="K534" s="156"/>
+      <c r="B534" s="167"/>
+      <c r="C534" s="157"/>
+      <c r="D534" s="157"/>
+      <c r="E534" s="157"/>
+      <c r="F534" s="157"/>
+      <c r="G534" s="157"/>
+      <c r="H534" s="157"/>
+      <c r="I534" s="174" t="s">
+        <v>1264</v>
+      </c>
+      <c r="J534" s="157"/>
+      <c r="K534" s="157"/>
     </row>
     <row r="535" ht="15.75" customHeight="1">
-      <c r="A535" s="166" t="s">
-        <v>1264</v>
-      </c>
-      <c r="B535" s="166"/>
-      <c r="C535" s="156"/>
-      <c r="D535" s="156"/>
-      <c r="E535" s="156"/>
-      <c r="F535" s="156"/>
-      <c r="G535" s="156"/>
-      <c r="H535" s="156"/>
-      <c r="I535" s="173" t="s">
+      <c r="A535" s="167" t="s">
         <v>1265</v>
       </c>
-      <c r="J535" s="156"/>
-      <c r="K535" s="156"/>
+      <c r="B535" s="167"/>
+      <c r="C535" s="157"/>
+      <c r="D535" s="157"/>
+      <c r="E535" s="157"/>
+      <c r="F535" s="157"/>
+      <c r="G535" s="157"/>
+      <c r="H535" s="157"/>
+      <c r="I535" s="174" t="s">
+        <v>1266</v>
+      </c>
+      <c r="J535" s="157"/>
+      <c r="K535" s="157"/>
     </row>
     <row r="536" ht="15.75" customHeight="1">
-      <c r="A536" s="166" t="s">
-        <v>1266</v>
-      </c>
-      <c r="B536" s="166"/>
-      <c r="C536" s="156"/>
-      <c r="D536" s="156"/>
-      <c r="E536" s="156"/>
-      <c r="F536" s="156"/>
-      <c r="G536" s="156"/>
-      <c r="H536" s="156"/>
-      <c r="I536" s="167" t="s">
+      <c r="A536" s="167" t="s">
         <v>1267</v>
       </c>
-      <c r="J536" s="156"/>
-      <c r="K536" s="156"/>
+      <c r="B536" s="167"/>
+      <c r="C536" s="157"/>
+      <c r="D536" s="157"/>
+      <c r="E536" s="157"/>
+      <c r="F536" s="157"/>
+      <c r="G536" s="157"/>
+      <c r="H536" s="157"/>
+      <c r="I536" s="168" t="s">
+        <v>1268</v>
+      </c>
+      <c r="J536" s="157"/>
+      <c r="K536" s="157"/>
     </row>
     <row r="537" ht="15.75" customHeight="1">
-      <c r="A537" s="166" t="s">
-        <v>1268</v>
-      </c>
-      <c r="B537" s="166"/>
-      <c r="C537" s="156"/>
-      <c r="D537" s="156"/>
-      <c r="E537" s="156"/>
-      <c r="F537" s="156"/>
-      <c r="G537" s="156"/>
-      <c r="H537" s="156"/>
-      <c r="I537" s="167" t="s">
+      <c r="A537" s="167" t="s">
         <v>1269</v>
       </c>
-      <c r="J537" s="156"/>
-      <c r="K537" s="156"/>
+      <c r="B537" s="167"/>
+      <c r="C537" s="157"/>
+      <c r="D537" s="157"/>
+      <c r="E537" s="157"/>
+      <c r="F537" s="157"/>
+      <c r="G537" s="157"/>
+      <c r="H537" s="157"/>
+      <c r="I537" s="168" t="s">
+        <v>1270</v>
+      </c>
+      <c r="J537" s="157"/>
+      <c r="K537" s="157"/>
     </row>
     <row r="538" ht="15.75" customHeight="1">
       <c r="A538" s="15" t="s">
-        <v>1270</v>
-      </c>
-      <c r="H538" s="156"/>
-      <c r="I538" s="174" t="s">
         <v>1271</v>
       </c>
-      <c r="J538" s="156"/>
-      <c r="K538" s="156"/>
+      <c r="H538" s="157"/>
+      <c r="I538" s="175" t="s">
+        <v>1272</v>
+      </c>
+      <c r="J538" s="157"/>
+      <c r="K538" s="157"/>
     </row>
     <row r="539" ht="15.75" customHeight="1">
       <c r="A539" s="15" t="s">
-        <v>1272</v>
+        <v>1273</v>
       </c>
       <c r="B539" s="15"/>
       <c r="C539" s="15"/>
@@ -13950,14 +13970,14 @@
       <c r="E539" s="15"/>
       <c r="F539" s="15"/>
       <c r="G539" s="15"/>
-      <c r="H539" s="156"/>
-      <c r="I539" s="174"/>
-      <c r="J539" s="156"/>
-      <c r="K539" s="156"/>
+      <c r="H539" s="157"/>
+      <c r="I539" s="175"/>
+      <c r="J539" s="157"/>
+      <c r="K539" s="157"/>
     </row>
     <row r="540" ht="15.75" customHeight="1">
       <c r="A540" s="15" t="s">
-        <v>1273</v>
+        <v>1274</v>
       </c>
       <c r="B540" s="15"/>
       <c r="C540" s="15"/>
@@ -13965,16 +13985,16 @@
       <c r="E540" s="15"/>
       <c r="F540" s="15"/>
       <c r="G540" s="15"/>
-      <c r="H540" s="156"/>
-      <c r="I540" s="167" t="s">
-        <v>1274</v>
-      </c>
-      <c r="J540" s="156"/>
-      <c r="K540" s="156"/>
+      <c r="H540" s="157"/>
+      <c r="I540" s="168" t="s">
+        <v>1275</v>
+      </c>
+      <c r="J540" s="157"/>
+      <c r="K540" s="157"/>
     </row>
     <row r="541" ht="15.75" customHeight="1">
       <c r="A541" s="15" t="s">
-        <v>1275</v>
+        <v>1276</v>
       </c>
       <c r="B541" s="15"/>
       <c r="C541" s="15"/>
@@ -13982,41 +14002,45 @@
       <c r="E541" s="15"/>
       <c r="F541" s="15"/>
       <c r="G541" s="15"/>
-      <c r="H541" s="156"/>
-      <c r="I541" s="167" t="s">
-        <v>1276</v>
-      </c>
-      <c r="J541" s="156"/>
-      <c r="K541" s="156"/>
+      <c r="H541" s="157"/>
+      <c r="I541" s="168" t="s">
+        <v>1277</v>
+      </c>
+      <c r="J541" s="157"/>
+      <c r="K541" s="157"/>
     </row>
     <row r="542" ht="15.75" customHeight="1">
       <c r="A542" s="15" t="s">
-        <v>1277</v>
+        <v>1278</v>
       </c>
       <c r="C542" s="15"/>
       <c r="D542" s="15"/>
       <c r="E542" s="15"/>
       <c r="F542" s="15"/>
       <c r="G542" s="15"/>
-      <c r="H542" s="156"/>
-      <c r="I542" s="168" t="s">
-        <v>1278</v>
-      </c>
-      <c r="J542" s="156"/>
-      <c r="K542" s="156"/>
+      <c r="H542" s="157"/>
+      <c r="I542" s="169" t="s">
+        <v>1279</v>
+      </c>
+      <c r="J542" s="157"/>
+      <c r="K542" s="157"/>
     </row>
     <row r="543" ht="15.75" customHeight="1">
-      <c r="A543" s="15"/>
+      <c r="A543" s="15" t="s">
+        <v>1280</v>
+      </c>
       <c r="B543" s="15"/>
       <c r="C543" s="15"/>
       <c r="D543" s="15"/>
       <c r="E543" s="15"/>
       <c r="F543" s="15"/>
       <c r="G543" s="15"/>
-      <c r="H543" s="156"/>
-      <c r="I543" s="174"/>
-      <c r="J543" s="156"/>
-      <c r="K543" s="156"/>
+      <c r="H543" s="157"/>
+      <c r="I543" s="168" t="s">
+        <v>1190</v>
+      </c>
+      <c r="J543" s="157"/>
+      <c r="K543" s="157"/>
     </row>
     <row r="544" ht="15.75" customHeight="1">
       <c r="A544" s="15"/>
@@ -14026,10 +14050,10 @@
       <c r="E544" s="15"/>
       <c r="F544" s="15"/>
       <c r="G544" s="15"/>
-      <c r="H544" s="156"/>
-      <c r="I544" s="174"/>
-      <c r="J544" s="156"/>
-      <c r="K544" s="156"/>
+      <c r="H544" s="157"/>
+      <c r="I544" s="175"/>
+      <c r="J544" s="157"/>
+      <c r="K544" s="157"/>
     </row>
     <row r="545" ht="15.75" customHeight="1">
       <c r="A545" s="15"/>
@@ -14039,10 +14063,10 @@
       <c r="E545" s="15"/>
       <c r="F545" s="15"/>
       <c r="G545" s="15"/>
-      <c r="H545" s="156"/>
-      <c r="I545" s="174"/>
-      <c r="J545" s="156"/>
-      <c r="K545" s="156"/>
+      <c r="H545" s="157"/>
+      <c r="I545" s="175"/>
+      <c r="J545" s="157"/>
+      <c r="K545" s="157"/>
     </row>
     <row r="546" ht="15.75" customHeight="1">
       <c r="A546" s="15"/>
@@ -14052,10 +14076,10 @@
       <c r="E546" s="15"/>
       <c r="F546" s="15"/>
       <c r="G546" s="15"/>
-      <c r="H546" s="156"/>
-      <c r="I546" s="174"/>
-      <c r="J546" s="156"/>
-      <c r="K546" s="156"/>
+      <c r="H546" s="157"/>
+      <c r="I546" s="175"/>
+      <c r="J546" s="157"/>
+      <c r="K546" s="157"/>
     </row>
     <row r="547" ht="15.75" customHeight="1">
       <c r="A547" s="15"/>
@@ -14065,10 +14089,10 @@
       <c r="E547" s="15"/>
       <c r="F547" s="15"/>
       <c r="G547" s="15"/>
-      <c r="H547" s="156"/>
-      <c r="I547" s="174"/>
-      <c r="J547" s="156"/>
-      <c r="K547" s="156"/>
+      <c r="H547" s="157"/>
+      <c r="I547" s="175"/>
+      <c r="J547" s="157"/>
+      <c r="K547" s="157"/>
     </row>
     <row r="548" ht="15.75" customHeight="1">
       <c r="A548" s="15"/>
@@ -14078,192 +14102,19 @@
       <c r="E548" s="15"/>
       <c r="F548" s="15"/>
       <c r="G548" s="15"/>
-      <c r="H548" s="156"/>
-      <c r="I548" s="174"/>
-      <c r="J548" s="156"/>
-      <c r="K548" s="156"/>
+      <c r="H548" s="157"/>
+      <c r="I548" s="175"/>
+      <c r="J548" s="157"/>
+      <c r="K548" s="157"/>
     </row>
   </sheetData>
   <mergeCells count="515">
-    <mergeCell ref="D120:G120"/>
-    <mergeCell ref="C110:G110"/>
-    <mergeCell ref="C114:G114"/>
-    <mergeCell ref="D63:G63"/>
-    <mergeCell ref="D62:G62"/>
-    <mergeCell ref="C79:G79"/>
-    <mergeCell ref="C91:G91"/>
-    <mergeCell ref="C86:G86"/>
-    <mergeCell ref="D64:G64"/>
-    <mergeCell ref="C69:G69"/>
-    <mergeCell ref="D68:G68"/>
-    <mergeCell ref="D67:G67"/>
-    <mergeCell ref="C70:G70"/>
-    <mergeCell ref="D72:G72"/>
-    <mergeCell ref="D125:G125"/>
-    <mergeCell ref="C60:G60"/>
-    <mergeCell ref="D121:G121"/>
-    <mergeCell ref="D122:G122"/>
-    <mergeCell ref="C109:G109"/>
-    <mergeCell ref="D61:G61"/>
-    <mergeCell ref="C92:G92"/>
-    <mergeCell ref="D73:G73"/>
-    <mergeCell ref="C108:G108"/>
-    <mergeCell ref="C99:G99"/>
-    <mergeCell ref="C100:G100"/>
-    <mergeCell ref="C103:G103"/>
-    <mergeCell ref="C102:G102"/>
-    <mergeCell ref="C104:G104"/>
-    <mergeCell ref="C105:G105"/>
-    <mergeCell ref="C106:G106"/>
-    <mergeCell ref="D96:G96"/>
-    <mergeCell ref="C98:G98"/>
-    <mergeCell ref="D97:G97"/>
-    <mergeCell ref="C95:G95"/>
-    <mergeCell ref="C94:G94"/>
-    <mergeCell ref="D65:G65"/>
-    <mergeCell ref="D66:G66"/>
-    <mergeCell ref="D71:G71"/>
-    <mergeCell ref="D74:G74"/>
-    <mergeCell ref="E75:G75"/>
-    <mergeCell ref="E76:G76"/>
-    <mergeCell ref="D88:G88"/>
-    <mergeCell ref="C85:G85"/>
-    <mergeCell ref="C78:G78"/>
-    <mergeCell ref="C77:G77"/>
-    <mergeCell ref="C87:G87"/>
-    <mergeCell ref="C90:G90"/>
-    <mergeCell ref="C89:G89"/>
-    <mergeCell ref="C80:G80"/>
-    <mergeCell ref="C81:G81"/>
-    <mergeCell ref="C83:G83"/>
-    <mergeCell ref="C82:G82"/>
-    <mergeCell ref="D54:G54"/>
-    <mergeCell ref="C55:G55"/>
-    <mergeCell ref="B56:G56"/>
-    <mergeCell ref="D49:G49"/>
-    <mergeCell ref="C50:G50"/>
-    <mergeCell ref="C59:G59"/>
-    <mergeCell ref="D48:G48"/>
-    <mergeCell ref="C58:G58"/>
-    <mergeCell ref="D53:G53"/>
-    <mergeCell ref="D52:G52"/>
-    <mergeCell ref="D51:G51"/>
-    <mergeCell ref="C57:G57"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="D28:G28"/>
-    <mergeCell ref="D30:G30"/>
-    <mergeCell ref="D29:G29"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="D31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="D25:G25"/>
-    <mergeCell ref="D24:G24"/>
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C44:G44"/>
-    <mergeCell ref="B45:G45"/>
-    <mergeCell ref="D47:G47"/>
-    <mergeCell ref="C41:G41"/>
-    <mergeCell ref="C40:G40"/>
-    <mergeCell ref="D39:G39"/>
-    <mergeCell ref="D38:G38"/>
-    <mergeCell ref="C46:G46"/>
-    <mergeCell ref="C42:G42"/>
-    <mergeCell ref="C43:G43"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="D191:G191"/>
-    <mergeCell ref="D190:G190"/>
-    <mergeCell ref="D185:G185"/>
-    <mergeCell ref="E184:G184"/>
-    <mergeCell ref="B195:G195"/>
-    <mergeCell ref="D192:G192"/>
-    <mergeCell ref="D186:G186"/>
-    <mergeCell ref="D187:G187"/>
-    <mergeCell ref="D188:G188"/>
-    <mergeCell ref="A194:G194"/>
-    <mergeCell ref="C461:G461"/>
-    <mergeCell ref="B466:G466"/>
-    <mergeCell ref="C505:G505"/>
-    <mergeCell ref="C506:G506"/>
-    <mergeCell ref="C450:G450"/>
-    <mergeCell ref="B451:G451"/>
-    <mergeCell ref="D448:G448"/>
-    <mergeCell ref="C449:G449"/>
-    <mergeCell ref="B458:G458"/>
-    <mergeCell ref="D303:G303"/>
-    <mergeCell ref="D301:G301"/>
-    <mergeCell ref="D302:G302"/>
-    <mergeCell ref="C304:G304"/>
-    <mergeCell ref="C305:G305"/>
-    <mergeCell ref="D306:G306"/>
-    <mergeCell ref="B285:G285"/>
-    <mergeCell ref="B284:G284"/>
-    <mergeCell ref="B297:G297"/>
-    <mergeCell ref="A283:G283"/>
-    <mergeCell ref="C313:G313"/>
-    <mergeCell ref="D292:G292"/>
-    <mergeCell ref="D369:G369"/>
-    <mergeCell ref="D368:G368"/>
-    <mergeCell ref="D367:G367"/>
-    <mergeCell ref="E360:G360"/>
-    <mergeCell ref="E371:G371"/>
-    <mergeCell ref="E370:G370"/>
-    <mergeCell ref="E363:G363"/>
-    <mergeCell ref="E364:G364"/>
-    <mergeCell ref="E362:G362"/>
-    <mergeCell ref="E365:G365"/>
-    <mergeCell ref="E366:G366"/>
-    <mergeCell ref="D355:G355"/>
-    <mergeCell ref="D356:G356"/>
-    <mergeCell ref="E358:G358"/>
-    <mergeCell ref="E357:G357"/>
-    <mergeCell ref="D307:G307"/>
-    <mergeCell ref="E310:G310"/>
-    <mergeCell ref="D348:G348"/>
-    <mergeCell ref="D349:G349"/>
-    <mergeCell ref="D344:G344"/>
-    <mergeCell ref="D342:G342"/>
-    <mergeCell ref="E359:G359"/>
-    <mergeCell ref="A401:G401"/>
-    <mergeCell ref="B398:G398"/>
-    <mergeCell ref="C399:G399"/>
-    <mergeCell ref="C390:G390"/>
-    <mergeCell ref="C395:G395"/>
-    <mergeCell ref="C387:G387"/>
-    <mergeCell ref="C388:G388"/>
-    <mergeCell ref="B382:G382"/>
-    <mergeCell ref="B383:G383"/>
-    <mergeCell ref="C403:G403"/>
-    <mergeCell ref="B402:G402"/>
-    <mergeCell ref="B389:G389"/>
-    <mergeCell ref="B281:G281"/>
-    <mergeCell ref="C276:G276"/>
-    <mergeCell ref="D280:G280"/>
-    <mergeCell ref="D279:G279"/>
+    <mergeCell ref="B518:G518"/>
+    <mergeCell ref="A529:G529"/>
+    <mergeCell ref="A530:G530"/>
+    <mergeCell ref="A538:G538"/>
+    <mergeCell ref="B509:G509"/>
+    <mergeCell ref="B508:G508"/>
     <mergeCell ref="B512:G512"/>
     <mergeCell ref="B513:G513"/>
     <mergeCell ref="B511:G511"/>
@@ -14271,30 +14122,15 @@
     <mergeCell ref="B515:G515"/>
     <mergeCell ref="B516:G516"/>
     <mergeCell ref="B517:G517"/>
-    <mergeCell ref="B518:G518"/>
-    <mergeCell ref="A529:G529"/>
-    <mergeCell ref="A530:G530"/>
-    <mergeCell ref="A538:G538"/>
-    <mergeCell ref="D294:G294"/>
-    <mergeCell ref="D293:G293"/>
-    <mergeCell ref="D361:G361"/>
-    <mergeCell ref="D373:G373"/>
-    <mergeCell ref="C374:G374"/>
-    <mergeCell ref="D372:G372"/>
-    <mergeCell ref="C409:G409"/>
-    <mergeCell ref="C414:G414"/>
-    <mergeCell ref="C413:G413"/>
-    <mergeCell ref="C412:G412"/>
-    <mergeCell ref="C411:G411"/>
-    <mergeCell ref="C410:G410"/>
-    <mergeCell ref="C507:G507"/>
-    <mergeCell ref="B509:G509"/>
-    <mergeCell ref="B508:G508"/>
+    <mergeCell ref="B510:G510"/>
+    <mergeCell ref="C505:G505"/>
     <mergeCell ref="C504:G504"/>
     <mergeCell ref="B502:G502"/>
     <mergeCell ref="C503:G503"/>
     <mergeCell ref="B486:G486"/>
     <mergeCell ref="C487:G487"/>
+    <mergeCell ref="C489:G489"/>
+    <mergeCell ref="C492:G492"/>
     <mergeCell ref="B485:G485"/>
     <mergeCell ref="B479:G479"/>
     <mergeCell ref="B480:G480"/>
@@ -14311,17 +14147,450 @@
     <mergeCell ref="C497:G497"/>
     <mergeCell ref="C500:G500"/>
     <mergeCell ref="C498:G498"/>
+    <mergeCell ref="C499:G499"/>
     <mergeCell ref="C501:G501"/>
-    <mergeCell ref="C499:G499"/>
     <mergeCell ref="C488:G488"/>
-    <mergeCell ref="C489:G489"/>
+    <mergeCell ref="C296:G296"/>
+    <mergeCell ref="C295:G295"/>
+    <mergeCell ref="D300:G300"/>
+    <mergeCell ref="C299:G299"/>
+    <mergeCell ref="D306:G306"/>
+    <mergeCell ref="B285:G285"/>
+    <mergeCell ref="A283:G283"/>
+    <mergeCell ref="B281:G281"/>
+    <mergeCell ref="C276:G276"/>
+    <mergeCell ref="D280:G280"/>
+    <mergeCell ref="C277:G277"/>
+    <mergeCell ref="C291:G291"/>
+    <mergeCell ref="C289:G289"/>
+    <mergeCell ref="C290:G290"/>
+    <mergeCell ref="B284:G284"/>
+    <mergeCell ref="C313:G313"/>
+    <mergeCell ref="D293:G293"/>
+    <mergeCell ref="C287:G287"/>
+    <mergeCell ref="C288:G288"/>
+    <mergeCell ref="C286:G286"/>
+    <mergeCell ref="C298:G298"/>
+    <mergeCell ref="B312:G312"/>
+    <mergeCell ref="D315:G315"/>
+    <mergeCell ref="D316:G316"/>
+    <mergeCell ref="D326:G326"/>
+    <mergeCell ref="D321:G321"/>
+    <mergeCell ref="D307:G307"/>
+    <mergeCell ref="E310:G310"/>
+    <mergeCell ref="E311:G311"/>
+    <mergeCell ref="D329:G329"/>
+    <mergeCell ref="D328:G328"/>
+    <mergeCell ref="D327:G327"/>
+    <mergeCell ref="D314:G314"/>
+    <mergeCell ref="E371:G371"/>
+    <mergeCell ref="E370:G370"/>
+    <mergeCell ref="E363:G363"/>
+    <mergeCell ref="E364:G364"/>
+    <mergeCell ref="E362:G362"/>
+    <mergeCell ref="E365:G365"/>
+    <mergeCell ref="D348:G348"/>
+    <mergeCell ref="D349:G349"/>
+    <mergeCell ref="D347:G347"/>
+    <mergeCell ref="D350:G350"/>
+    <mergeCell ref="D336:G336"/>
+    <mergeCell ref="D335:G335"/>
+    <mergeCell ref="D353:G353"/>
+    <mergeCell ref="D352:G352"/>
+    <mergeCell ref="D351:G351"/>
+    <mergeCell ref="E366:G366"/>
+    <mergeCell ref="D355:G355"/>
+    <mergeCell ref="D356:G356"/>
+    <mergeCell ref="E358:G358"/>
+    <mergeCell ref="E357:G357"/>
+    <mergeCell ref="D361:G361"/>
+    <mergeCell ref="E354:G354"/>
+    <mergeCell ref="D308:G308"/>
+    <mergeCell ref="D309:G309"/>
+    <mergeCell ref="D332:G332"/>
+    <mergeCell ref="D331:G331"/>
+    <mergeCell ref="D367:G367"/>
+    <mergeCell ref="E360:G360"/>
+    <mergeCell ref="E359:G359"/>
+    <mergeCell ref="D341:G341"/>
+    <mergeCell ref="D343:G343"/>
+    <mergeCell ref="D338:G338"/>
+    <mergeCell ref="C346:G346"/>
+    <mergeCell ref="B297:G297"/>
+    <mergeCell ref="D294:G294"/>
+    <mergeCell ref="C416:G416"/>
+    <mergeCell ref="C415:G415"/>
+    <mergeCell ref="D266:G266"/>
+    <mergeCell ref="D267:G267"/>
+    <mergeCell ref="C269:G269"/>
+    <mergeCell ref="D268:G268"/>
+    <mergeCell ref="D271:G271"/>
+    <mergeCell ref="D270:G270"/>
+    <mergeCell ref="D272:G272"/>
+    <mergeCell ref="D279:G279"/>
+    <mergeCell ref="C278:G278"/>
+    <mergeCell ref="D275:G275"/>
+    <mergeCell ref="C274:G274"/>
+    <mergeCell ref="D273:G273"/>
+    <mergeCell ref="D324:G324"/>
+    <mergeCell ref="D323:G323"/>
+    <mergeCell ref="C304:G304"/>
+    <mergeCell ref="C305:G305"/>
+    <mergeCell ref="D319:G319"/>
+    <mergeCell ref="D320:G320"/>
+    <mergeCell ref="D317:G317"/>
+    <mergeCell ref="D318:G318"/>
+    <mergeCell ref="D325:G325"/>
+    <mergeCell ref="D322:G322"/>
+    <mergeCell ref="D67:G67"/>
+    <mergeCell ref="C70:G70"/>
+    <mergeCell ref="E75:G75"/>
+    <mergeCell ref="E76:G76"/>
+    <mergeCell ref="C79:G79"/>
+    <mergeCell ref="C78:G78"/>
+    <mergeCell ref="C77:G77"/>
+    <mergeCell ref="C80:G80"/>
+    <mergeCell ref="C81:G81"/>
+    <mergeCell ref="C83:G83"/>
+    <mergeCell ref="C82:G82"/>
+    <mergeCell ref="C59:G59"/>
+    <mergeCell ref="C58:G58"/>
+    <mergeCell ref="C57:G57"/>
+    <mergeCell ref="D62:G62"/>
+    <mergeCell ref="C86:G86"/>
+    <mergeCell ref="D72:G72"/>
+    <mergeCell ref="C60:G60"/>
+    <mergeCell ref="D61:G61"/>
+    <mergeCell ref="D71:G71"/>
+    <mergeCell ref="C85:G85"/>
+    <mergeCell ref="C111:G111"/>
+    <mergeCell ref="C112:G112"/>
+    <mergeCell ref="C114:G114"/>
+    <mergeCell ref="C108:G108"/>
+    <mergeCell ref="C119:G119"/>
+    <mergeCell ref="D116:G116"/>
+    <mergeCell ref="D117:G117"/>
+    <mergeCell ref="D118:G118"/>
+    <mergeCell ref="C115:G115"/>
+    <mergeCell ref="D63:G63"/>
+    <mergeCell ref="D64:G64"/>
+    <mergeCell ref="C69:G69"/>
+    <mergeCell ref="D68:G68"/>
+    <mergeCell ref="C110:G110"/>
+    <mergeCell ref="C109:G109"/>
+    <mergeCell ref="D65:G65"/>
+    <mergeCell ref="D66:G66"/>
+    <mergeCell ref="D73:G73"/>
+    <mergeCell ref="D74:G74"/>
+    <mergeCell ref="D88:G88"/>
+    <mergeCell ref="C87:G87"/>
+    <mergeCell ref="C90:G90"/>
+    <mergeCell ref="C89:G89"/>
+    <mergeCell ref="D171:G171"/>
+    <mergeCell ref="E172:G172"/>
+    <mergeCell ref="C161:G161"/>
+    <mergeCell ref="D160:G160"/>
+    <mergeCell ref="D158:G158"/>
+    <mergeCell ref="D159:G159"/>
+    <mergeCell ref="D157:G157"/>
+    <mergeCell ref="D156:G156"/>
+    <mergeCell ref="D128:G128"/>
+    <mergeCell ref="D129:G129"/>
+    <mergeCell ref="D133:G133"/>
+    <mergeCell ref="C127:G127"/>
+    <mergeCell ref="C135:G135"/>
+    <mergeCell ref="C134:G134"/>
+    <mergeCell ref="D130:G130"/>
+    <mergeCell ref="E184:G184"/>
+    <mergeCell ref="D165:G165"/>
+    <mergeCell ref="E177:G177"/>
+    <mergeCell ref="E176:G176"/>
+    <mergeCell ref="D181:G181"/>
+    <mergeCell ref="E180:G180"/>
+    <mergeCell ref="C163:G163"/>
+    <mergeCell ref="D120:G120"/>
+    <mergeCell ref="D121:G121"/>
+    <mergeCell ref="D122:G122"/>
+    <mergeCell ref="D188:G188"/>
+    <mergeCell ref="E183:G183"/>
+    <mergeCell ref="D153:G153"/>
+    <mergeCell ref="D131:G131"/>
+    <mergeCell ref="D178:G178"/>
+    <mergeCell ref="E179:G179"/>
+    <mergeCell ref="C138:G138"/>
+    <mergeCell ref="C139:G139"/>
+    <mergeCell ref="C136:G136"/>
+    <mergeCell ref="C137:G137"/>
+    <mergeCell ref="E152:G152"/>
+    <mergeCell ref="C155:G155"/>
+    <mergeCell ref="E147:G147"/>
+    <mergeCell ref="E150:G150"/>
+    <mergeCell ref="E149:G149"/>
+    <mergeCell ref="E148:G148"/>
+    <mergeCell ref="E151:G151"/>
+    <mergeCell ref="C141:G141"/>
+    <mergeCell ref="C142:G142"/>
+    <mergeCell ref="C144:G144"/>
+    <mergeCell ref="D125:G125"/>
+    <mergeCell ref="D124:G124"/>
+    <mergeCell ref="D140:G140"/>
+    <mergeCell ref="D132:G132"/>
+    <mergeCell ref="D123:G123"/>
+    <mergeCell ref="D126:G126"/>
+    <mergeCell ref="C412:G412"/>
+    <mergeCell ref="C411:G411"/>
+    <mergeCell ref="C409:G409"/>
+    <mergeCell ref="C406:G406"/>
+    <mergeCell ref="C407:G407"/>
+    <mergeCell ref="B404:G404"/>
+    <mergeCell ref="B405:G405"/>
+    <mergeCell ref="C388:G388"/>
+    <mergeCell ref="C391:G391"/>
+    <mergeCell ref="C387:G387"/>
+    <mergeCell ref="C403:G403"/>
+    <mergeCell ref="B402:G402"/>
+    <mergeCell ref="C414:G414"/>
+    <mergeCell ref="C413:G413"/>
+    <mergeCell ref="C410:G410"/>
+    <mergeCell ref="B408:G408"/>
+    <mergeCell ref="B400:G400"/>
+    <mergeCell ref="C441:G441"/>
+    <mergeCell ref="C442:G442"/>
+    <mergeCell ref="C440:G440"/>
+    <mergeCell ref="B439:G439"/>
+    <mergeCell ref="B438:G438"/>
+    <mergeCell ref="A437:G437"/>
+    <mergeCell ref="C450:G450"/>
+    <mergeCell ref="D448:G448"/>
+    <mergeCell ref="C449:G449"/>
+    <mergeCell ref="C446:G446"/>
+    <mergeCell ref="C443:G443"/>
+    <mergeCell ref="C444:G444"/>
+    <mergeCell ref="C445:G445"/>
+    <mergeCell ref="D333:G333"/>
+    <mergeCell ref="D334:G334"/>
+    <mergeCell ref="D344:G344"/>
+    <mergeCell ref="D342:G342"/>
+    <mergeCell ref="D339:G339"/>
+    <mergeCell ref="D340:G340"/>
+    <mergeCell ref="E345:G345"/>
+    <mergeCell ref="D330:G330"/>
+    <mergeCell ref="D337:G337"/>
+    <mergeCell ref="B422:G422"/>
+    <mergeCell ref="C424:G424"/>
+    <mergeCell ref="C423:G423"/>
+    <mergeCell ref="B418:G418"/>
+    <mergeCell ref="C419:G419"/>
+    <mergeCell ref="C428:G428"/>
+    <mergeCell ref="C426:G426"/>
+    <mergeCell ref="C427:G427"/>
+    <mergeCell ref="C421:G421"/>
+    <mergeCell ref="C420:G420"/>
+    <mergeCell ref="B429:G429"/>
+    <mergeCell ref="C432:G432"/>
+    <mergeCell ref="B434:G434"/>
+    <mergeCell ref="B433:G433"/>
+    <mergeCell ref="C417:G417"/>
+    <mergeCell ref="C430:G430"/>
+    <mergeCell ref="C425:G425"/>
+    <mergeCell ref="C431:G431"/>
+    <mergeCell ref="C374:G374"/>
+    <mergeCell ref="D378:G378"/>
+    <mergeCell ref="D377:G377"/>
+    <mergeCell ref="D376:G376"/>
+    <mergeCell ref="D375:G375"/>
+    <mergeCell ref="D368:G368"/>
+    <mergeCell ref="A401:G401"/>
+    <mergeCell ref="C399:G399"/>
+    <mergeCell ref="C395:G395"/>
+    <mergeCell ref="B389:G389"/>
+    <mergeCell ref="C396:G396"/>
+    <mergeCell ref="B385:G385"/>
+    <mergeCell ref="B382:G382"/>
+    <mergeCell ref="B383:G383"/>
+    <mergeCell ref="D369:G369"/>
+    <mergeCell ref="D373:G373"/>
+    <mergeCell ref="D372:G372"/>
+    <mergeCell ref="D379:G379"/>
+    <mergeCell ref="D381:G381"/>
+    <mergeCell ref="D380:G380"/>
+    <mergeCell ref="B398:G398"/>
+    <mergeCell ref="B397:G397"/>
+    <mergeCell ref="C393:G393"/>
+    <mergeCell ref="B394:G394"/>
+    <mergeCell ref="C386:G386"/>
+    <mergeCell ref="C384:G384"/>
+    <mergeCell ref="C390:G390"/>
+    <mergeCell ref="C392:G392"/>
+    <mergeCell ref="D257:G257"/>
+    <mergeCell ref="D265:G265"/>
+    <mergeCell ref="D264:G264"/>
+    <mergeCell ref="D263:G263"/>
+    <mergeCell ref="D262:G262"/>
+    <mergeCell ref="D258:G258"/>
+    <mergeCell ref="D261:G261"/>
+    <mergeCell ref="C229:G229"/>
+    <mergeCell ref="C231:G231"/>
+    <mergeCell ref="C230:G230"/>
+    <mergeCell ref="D237:G237"/>
+    <mergeCell ref="C234:G234"/>
+    <mergeCell ref="D236:G236"/>
+    <mergeCell ref="C235:G235"/>
+    <mergeCell ref="C233:G233"/>
+    <mergeCell ref="C232:G232"/>
+    <mergeCell ref="D250:G250"/>
+    <mergeCell ref="D251:G251"/>
+    <mergeCell ref="D241:G241"/>
+    <mergeCell ref="D243:G243"/>
+    <mergeCell ref="D244:G244"/>
+    <mergeCell ref="D245:G245"/>
+    <mergeCell ref="C227:G227"/>
+    <mergeCell ref="C222:G222"/>
+    <mergeCell ref="C223:G223"/>
+    <mergeCell ref="C228:G228"/>
+    <mergeCell ref="C253:G253"/>
+    <mergeCell ref="C238:G238"/>
+    <mergeCell ref="D239:G239"/>
+    <mergeCell ref="C204:G204"/>
+    <mergeCell ref="B203:G203"/>
+    <mergeCell ref="C202:G202"/>
+    <mergeCell ref="C197:G197"/>
+    <mergeCell ref="B198:G198"/>
+    <mergeCell ref="C196:G196"/>
+    <mergeCell ref="C200:G200"/>
+    <mergeCell ref="C201:G201"/>
+    <mergeCell ref="C199:G199"/>
+    <mergeCell ref="D146:G146"/>
+    <mergeCell ref="D145:G145"/>
+    <mergeCell ref="B154:G154"/>
+    <mergeCell ref="B143:G143"/>
+    <mergeCell ref="D170:G170"/>
+    <mergeCell ref="C168:G168"/>
+    <mergeCell ref="D185:G185"/>
+    <mergeCell ref="E182:G182"/>
+    <mergeCell ref="C189:G189"/>
+    <mergeCell ref="C174:G174"/>
+    <mergeCell ref="D175:G175"/>
+    <mergeCell ref="D190:G190"/>
+    <mergeCell ref="D205:G205"/>
+    <mergeCell ref="D206:G206"/>
+    <mergeCell ref="D211:G211"/>
+    <mergeCell ref="D212:G212"/>
+    <mergeCell ref="D214:G214"/>
+    <mergeCell ref="D213:G213"/>
+    <mergeCell ref="C468:G468"/>
+    <mergeCell ref="C467:G467"/>
+    <mergeCell ref="C453:G453"/>
+    <mergeCell ref="C452:G452"/>
+    <mergeCell ref="C456:G456"/>
+    <mergeCell ref="C457:G457"/>
+    <mergeCell ref="C218:G218"/>
+    <mergeCell ref="C217:G217"/>
+    <mergeCell ref="B220:G220"/>
+    <mergeCell ref="B221:G221"/>
+    <mergeCell ref="B224:G224"/>
+    <mergeCell ref="B225:G225"/>
+    <mergeCell ref="B226:G226"/>
+    <mergeCell ref="C210:G210"/>
+    <mergeCell ref="C216:G216"/>
+    <mergeCell ref="C215:G215"/>
+    <mergeCell ref="B451:G451"/>
+    <mergeCell ref="C447:G447"/>
+    <mergeCell ref="D292:G292"/>
+    <mergeCell ref="D252:G252"/>
+    <mergeCell ref="D254:G254"/>
+    <mergeCell ref="D260:G260"/>
+    <mergeCell ref="D259:G259"/>
+    <mergeCell ref="D256:G256"/>
+    <mergeCell ref="D255:G255"/>
+    <mergeCell ref="D249:G249"/>
+    <mergeCell ref="D248:G248"/>
+    <mergeCell ref="D247:G247"/>
+    <mergeCell ref="D246:G246"/>
+    <mergeCell ref="D242:G242"/>
+    <mergeCell ref="D240:G240"/>
+    <mergeCell ref="C105:G105"/>
+    <mergeCell ref="C106:G106"/>
+    <mergeCell ref="B107:G107"/>
+    <mergeCell ref="B113:G113"/>
+    <mergeCell ref="C99:G99"/>
+    <mergeCell ref="C98:G98"/>
+    <mergeCell ref="D96:G96"/>
+    <mergeCell ref="C95:G95"/>
+    <mergeCell ref="C94:G94"/>
+    <mergeCell ref="B93:G93"/>
+    <mergeCell ref="C91:G91"/>
+    <mergeCell ref="B84:G84"/>
+    <mergeCell ref="C92:G92"/>
+    <mergeCell ref="C100:G100"/>
+    <mergeCell ref="C103:G103"/>
+    <mergeCell ref="C102:G102"/>
+    <mergeCell ref="C104:G104"/>
+    <mergeCell ref="D97:G97"/>
+    <mergeCell ref="B101:G101"/>
+    <mergeCell ref="D54:G54"/>
+    <mergeCell ref="C55:G55"/>
+    <mergeCell ref="B56:G56"/>
+    <mergeCell ref="D49:G49"/>
+    <mergeCell ref="C50:G50"/>
+    <mergeCell ref="D53:G53"/>
+    <mergeCell ref="B45:G45"/>
+    <mergeCell ref="C46:G46"/>
+    <mergeCell ref="C40:G40"/>
+    <mergeCell ref="D39:G39"/>
+    <mergeCell ref="D38:G38"/>
+    <mergeCell ref="C42:G42"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="D52:G52"/>
+    <mergeCell ref="D51:G51"/>
+    <mergeCell ref="D28:G28"/>
+    <mergeCell ref="D29:G29"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C43:G43"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="D25:G25"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="D30:G30"/>
+    <mergeCell ref="D31:G31"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="D48:G48"/>
+    <mergeCell ref="D47:G47"/>
+    <mergeCell ref="C44:G44"/>
+    <mergeCell ref="C41:G41"/>
+    <mergeCell ref="D24:G24"/>
+    <mergeCell ref="C23:G23"/>
     <mergeCell ref="C459:G459"/>
     <mergeCell ref="C460:G460"/>
     <mergeCell ref="C454:G454"/>
     <mergeCell ref="C455:G455"/>
     <mergeCell ref="B478:G478"/>
     <mergeCell ref="B477:G477"/>
-    <mergeCell ref="C465:G465"/>
+    <mergeCell ref="A476:G476"/>
+    <mergeCell ref="C461:G461"/>
     <mergeCell ref="B462:G462"/>
     <mergeCell ref="C463:G463"/>
     <mergeCell ref="C464:G464"/>
@@ -14331,275 +14600,30 @@
     <mergeCell ref="C472:G472"/>
     <mergeCell ref="B469:G469"/>
     <mergeCell ref="C470:G470"/>
-    <mergeCell ref="C468:G468"/>
-    <mergeCell ref="C467:G467"/>
-    <mergeCell ref="C453:G453"/>
-    <mergeCell ref="C452:G452"/>
-    <mergeCell ref="C456:G456"/>
-    <mergeCell ref="C457:G457"/>
-    <mergeCell ref="C446:G446"/>
-    <mergeCell ref="A476:G476"/>
-    <mergeCell ref="C443:G443"/>
-    <mergeCell ref="C444:G444"/>
-    <mergeCell ref="C445:G445"/>
-    <mergeCell ref="B429:G429"/>
-    <mergeCell ref="C432:G432"/>
-    <mergeCell ref="B434:G434"/>
-    <mergeCell ref="B433:G433"/>
-    <mergeCell ref="C441:G441"/>
-    <mergeCell ref="C442:G442"/>
-    <mergeCell ref="C440:G440"/>
-    <mergeCell ref="C428:G428"/>
-    <mergeCell ref="B439:G439"/>
-    <mergeCell ref="B438:G438"/>
-    <mergeCell ref="A437:G437"/>
-    <mergeCell ref="D378:G378"/>
-    <mergeCell ref="D379:G379"/>
-    <mergeCell ref="D377:G377"/>
-    <mergeCell ref="E354:G354"/>
-    <mergeCell ref="D353:G353"/>
-    <mergeCell ref="D376:G376"/>
-    <mergeCell ref="D375:G375"/>
-    <mergeCell ref="D381:G381"/>
-    <mergeCell ref="D380:G380"/>
-    <mergeCell ref="D352:G352"/>
-    <mergeCell ref="D339:G339"/>
-    <mergeCell ref="D340:G340"/>
-    <mergeCell ref="D347:G347"/>
-    <mergeCell ref="E345:G345"/>
-    <mergeCell ref="D350:G350"/>
-    <mergeCell ref="D351:G351"/>
-    <mergeCell ref="D330:G330"/>
-    <mergeCell ref="D337:G337"/>
-    <mergeCell ref="D333:G333"/>
-    <mergeCell ref="D334:G334"/>
-    <mergeCell ref="D341:G341"/>
-    <mergeCell ref="D343:G343"/>
-    <mergeCell ref="D338:G338"/>
-    <mergeCell ref="C393:G393"/>
-    <mergeCell ref="B397:G397"/>
-    <mergeCell ref="C396:G396"/>
-    <mergeCell ref="B394:G394"/>
-    <mergeCell ref="C406:G406"/>
-    <mergeCell ref="B404:G404"/>
-    <mergeCell ref="B405:G405"/>
-    <mergeCell ref="B418:G418"/>
-    <mergeCell ref="C416:G416"/>
-    <mergeCell ref="C417:G417"/>
-    <mergeCell ref="C415:G415"/>
-    <mergeCell ref="B422:G422"/>
-    <mergeCell ref="C424:G424"/>
-    <mergeCell ref="C423:G423"/>
-    <mergeCell ref="C430:G430"/>
-    <mergeCell ref="C419:G419"/>
-    <mergeCell ref="C421:G421"/>
-    <mergeCell ref="C426:G426"/>
-    <mergeCell ref="C425:G425"/>
-    <mergeCell ref="C427:G427"/>
-    <mergeCell ref="C420:G420"/>
-    <mergeCell ref="C407:G407"/>
-    <mergeCell ref="B408:G408"/>
-    <mergeCell ref="C431:G431"/>
-    <mergeCell ref="C386:G386"/>
-    <mergeCell ref="C384:G384"/>
-    <mergeCell ref="B385:G385"/>
-    <mergeCell ref="C392:G392"/>
-    <mergeCell ref="C391:G391"/>
-    <mergeCell ref="B400:G400"/>
-    <mergeCell ref="D326:G326"/>
-    <mergeCell ref="E311:G311"/>
-    <mergeCell ref="D266:G266"/>
-    <mergeCell ref="D267:G267"/>
-    <mergeCell ref="D329:G329"/>
-    <mergeCell ref="D328:G328"/>
-    <mergeCell ref="D327:G327"/>
-    <mergeCell ref="D275:G275"/>
-    <mergeCell ref="C346:G346"/>
-    <mergeCell ref="D165:G165"/>
     <mergeCell ref="D167:G167"/>
+    <mergeCell ref="D169:G169"/>
+    <mergeCell ref="D191:G191"/>
+    <mergeCell ref="B195:G195"/>
+    <mergeCell ref="D192:G192"/>
+    <mergeCell ref="A194:G194"/>
     <mergeCell ref="D166:G166"/>
     <mergeCell ref="D164:G164"/>
     <mergeCell ref="D173:G173"/>
-    <mergeCell ref="D169:G169"/>
-    <mergeCell ref="D171:G171"/>
-    <mergeCell ref="E172:G172"/>
-    <mergeCell ref="D170:G170"/>
-    <mergeCell ref="E177:G177"/>
-    <mergeCell ref="E176:G176"/>
-    <mergeCell ref="D140:G140"/>
-    <mergeCell ref="D205:G205"/>
-    <mergeCell ref="D206:G206"/>
-    <mergeCell ref="D211:G211"/>
-    <mergeCell ref="D212:G212"/>
-    <mergeCell ref="D214:G214"/>
-    <mergeCell ref="D213:G213"/>
-    <mergeCell ref="D181:G181"/>
-    <mergeCell ref="E180:G180"/>
-    <mergeCell ref="C204:G204"/>
-    <mergeCell ref="B203:G203"/>
-    <mergeCell ref="C197:G197"/>
-    <mergeCell ref="B198:G198"/>
-    <mergeCell ref="C196:G196"/>
-    <mergeCell ref="C202:G202"/>
-    <mergeCell ref="C200:G200"/>
-    <mergeCell ref="C201:G201"/>
-    <mergeCell ref="C199:G199"/>
-    <mergeCell ref="D146:G146"/>
-    <mergeCell ref="D145:G145"/>
-    <mergeCell ref="C163:G163"/>
-    <mergeCell ref="C168:G168"/>
-    <mergeCell ref="D178:G178"/>
-    <mergeCell ref="E182:G182"/>
-    <mergeCell ref="C189:G189"/>
-    <mergeCell ref="C174:G174"/>
-    <mergeCell ref="D175:G175"/>
-    <mergeCell ref="E183:G183"/>
-    <mergeCell ref="E179:G179"/>
-    <mergeCell ref="C229:G229"/>
-    <mergeCell ref="C227:G227"/>
-    <mergeCell ref="C222:G222"/>
-    <mergeCell ref="C223:G223"/>
-    <mergeCell ref="C228:G228"/>
-    <mergeCell ref="E152:G152"/>
-    <mergeCell ref="E147:G147"/>
-    <mergeCell ref="E150:G150"/>
-    <mergeCell ref="E149:G149"/>
-    <mergeCell ref="E148:G148"/>
-    <mergeCell ref="E151:G151"/>
-    <mergeCell ref="B154:G154"/>
-    <mergeCell ref="D153:G153"/>
-    <mergeCell ref="C141:G141"/>
-    <mergeCell ref="C138:G138"/>
-    <mergeCell ref="C139:G139"/>
-    <mergeCell ref="B143:G143"/>
-    <mergeCell ref="C142:G142"/>
-    <mergeCell ref="C155:G155"/>
-    <mergeCell ref="C144:G144"/>
-    <mergeCell ref="C136:G136"/>
-    <mergeCell ref="C137:G137"/>
-    <mergeCell ref="C119:G119"/>
-    <mergeCell ref="D116:G116"/>
-    <mergeCell ref="D117:G117"/>
-    <mergeCell ref="D118:G118"/>
-    <mergeCell ref="D124:G124"/>
-    <mergeCell ref="D123:G123"/>
-    <mergeCell ref="C115:G115"/>
-    <mergeCell ref="C111:G111"/>
-    <mergeCell ref="C112:G112"/>
-    <mergeCell ref="B107:G107"/>
-    <mergeCell ref="B93:G93"/>
-    <mergeCell ref="B113:G113"/>
-    <mergeCell ref="B101:G101"/>
-    <mergeCell ref="B84:G84"/>
-    <mergeCell ref="D132:G132"/>
-    <mergeCell ref="D131:G131"/>
-    <mergeCell ref="D126:G126"/>
-    <mergeCell ref="D128:G128"/>
-    <mergeCell ref="D129:G129"/>
-    <mergeCell ref="D133:G133"/>
-    <mergeCell ref="C127:G127"/>
-    <mergeCell ref="C135:G135"/>
-    <mergeCell ref="C134:G134"/>
-    <mergeCell ref="D130:G130"/>
     <mergeCell ref="B162:G162"/>
-    <mergeCell ref="C161:G161"/>
-    <mergeCell ref="D160:G160"/>
-    <mergeCell ref="D158:G158"/>
-    <mergeCell ref="D159:G159"/>
-    <mergeCell ref="D157:G157"/>
-    <mergeCell ref="D156:G156"/>
-    <mergeCell ref="C218:G218"/>
-    <mergeCell ref="C217:G217"/>
-    <mergeCell ref="B220:G220"/>
-    <mergeCell ref="B221:G221"/>
-    <mergeCell ref="B224:G224"/>
-    <mergeCell ref="B225:G225"/>
-    <mergeCell ref="B226:G226"/>
+    <mergeCell ref="D186:G186"/>
+    <mergeCell ref="B466:G466"/>
+    <mergeCell ref="C506:G506"/>
+    <mergeCell ref="B458:G458"/>
+    <mergeCell ref="C507:G507"/>
+    <mergeCell ref="C465:G465"/>
+    <mergeCell ref="C219:G219"/>
+    <mergeCell ref="D187:G187"/>
+    <mergeCell ref="D303:G303"/>
+    <mergeCell ref="D301:G301"/>
+    <mergeCell ref="D302:G302"/>
     <mergeCell ref="D207:G207"/>
     <mergeCell ref="E208:G208"/>
-    <mergeCell ref="C210:G210"/>
     <mergeCell ref="D209:G209"/>
-    <mergeCell ref="C216:G216"/>
-    <mergeCell ref="C215:G215"/>
-    <mergeCell ref="C219:G219"/>
-    <mergeCell ref="C278:G278"/>
-    <mergeCell ref="C277:G277"/>
-    <mergeCell ref="C269:G269"/>
-    <mergeCell ref="D268:G268"/>
-    <mergeCell ref="C274:G274"/>
-    <mergeCell ref="D271:G271"/>
-    <mergeCell ref="D270:G270"/>
-    <mergeCell ref="D272:G272"/>
-    <mergeCell ref="D273:G273"/>
-    <mergeCell ref="C289:G289"/>
-    <mergeCell ref="C287:G287"/>
-    <mergeCell ref="C288:G288"/>
-    <mergeCell ref="C286:G286"/>
-    <mergeCell ref="C296:G296"/>
-    <mergeCell ref="C295:G295"/>
-    <mergeCell ref="D308:G308"/>
-    <mergeCell ref="D309:G309"/>
-    <mergeCell ref="D300:G300"/>
-    <mergeCell ref="C299:G299"/>
-    <mergeCell ref="C298:G298"/>
-    <mergeCell ref="C290:G290"/>
-    <mergeCell ref="C291:G291"/>
-    <mergeCell ref="C492:G492"/>
-    <mergeCell ref="C447:G447"/>
-    <mergeCell ref="D315:G315"/>
-    <mergeCell ref="D316:G316"/>
-    <mergeCell ref="D319:G319"/>
-    <mergeCell ref="D320:G320"/>
-    <mergeCell ref="D317:G317"/>
-    <mergeCell ref="D318:G318"/>
-    <mergeCell ref="D325:G325"/>
-    <mergeCell ref="D324:G324"/>
-    <mergeCell ref="D323:G323"/>
-    <mergeCell ref="D322:G322"/>
-    <mergeCell ref="D332:G332"/>
-    <mergeCell ref="D331:G331"/>
-    <mergeCell ref="D336:G336"/>
-    <mergeCell ref="D335:G335"/>
-    <mergeCell ref="B312:G312"/>
-    <mergeCell ref="B510:G510"/>
-    <mergeCell ref="D314:G314"/>
-    <mergeCell ref="D321:G321"/>
-    <mergeCell ref="D252:G252"/>
-    <mergeCell ref="D256:G256"/>
-    <mergeCell ref="D255:G255"/>
-    <mergeCell ref="D254:G254"/>
-    <mergeCell ref="D260:G260"/>
-    <mergeCell ref="D259:G259"/>
-    <mergeCell ref="D249:G249"/>
-    <mergeCell ref="D248:G248"/>
-    <mergeCell ref="D247:G247"/>
-    <mergeCell ref="D246:G246"/>
-    <mergeCell ref="D242:G242"/>
-    <mergeCell ref="D240:G240"/>
-    <mergeCell ref="D241:G241"/>
-    <mergeCell ref="D257:G257"/>
-    <mergeCell ref="C253:G253"/>
-    <mergeCell ref="D265:G265"/>
-    <mergeCell ref="D264:G264"/>
-    <mergeCell ref="D237:G237"/>
-    <mergeCell ref="C231:G231"/>
-    <mergeCell ref="C238:G238"/>
-    <mergeCell ref="C234:G234"/>
-    <mergeCell ref="C230:G230"/>
-    <mergeCell ref="C233:G233"/>
-    <mergeCell ref="C232:G232"/>
-    <mergeCell ref="D236:G236"/>
-    <mergeCell ref="C235:G235"/>
-    <mergeCell ref="D250:G250"/>
-    <mergeCell ref="D251:G251"/>
-    <mergeCell ref="D239:G239"/>
-    <mergeCell ref="D243:G243"/>
-    <mergeCell ref="D244:G244"/>
-    <mergeCell ref="D245:G245"/>
-    <mergeCell ref="D263:G263"/>
-    <mergeCell ref="D262:G262"/>
-    <mergeCell ref="D258:G258"/>
-    <mergeCell ref="D261:G261"/>
   </mergeCells>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>

</xml_diff>